<commit_message>
third commit with time functions in ipynb
</commit_message>
<xml_diff>
--- a/billing.xlsx
+++ b/billing.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haosenhe/PyFolder/Programs/nova-data-processing-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908AF329-904C-234A-8CE3-161134B97B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8586DB16-48D3-B94E-A04D-94FE0F16EFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="500" windowWidth="24960" windowHeight="21100" activeTab="1" xr2:uid="{2580F89A-B4FE-4711-8C11-BBD44F6FB879}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{2580F89A-B4FE-4711-8C11-BBD44F6FB879}"/>
   </bookViews>
   <sheets>
-    <sheet name="Billing &amp; Wage Rates by Shift" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Non-manager Rates" sheetId="3" r:id="rId1"/>
+    <sheet name="Manager Rates" sheetId="4" r:id="rId2"/>
     <sheet name="Person-Specific Pay Rates" sheetId="2" r:id="rId3"/>
+    <sheet name="Billing &amp; Wage Rates by Shift" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="114">
   <si>
     <t>HSS1</t>
   </si>
@@ -144,6 +145,9 @@
   </si>
   <si>
     <t>Wages paid by county; only used to calculate blended overtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*APPROVED HOLIDAY HOURS start at 7 a.m. and end at 11 p.m. on Easter Sunday, Thanksgiving, Christmas Eve, Christmas Day, and New Year’s Day.  Approved holiday hours also include the swing shift on New Year’s Eve (i.e., 11 p.m. on December 31st to 7 a.m. on January 1st.) NON-EXEMPT EMPLOYEES working Approved Holiday Hours will be paid "time and a half" for each Approved Holiday Hour worked.  EXEMPT EMPLOYEES working Approved Holiday Hours in a week when they are salaried will be paid a holiday bonus (50% of their nonexempt hourly rate) for each Holiday Hour worked during that week. </t>
   </si>
   <si>
     <r>
@@ -429,34 +433,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">MANAGERS' SALARY </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PAID BIMONTHLY</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (WHEN EXEMPT)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>MANAGERS' SALARY</t>
     </r>
     <r>
@@ -483,6 +459,61 @@
       <t xml:space="preserve"> (WHEN EXEMPT)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MANAGERS' SALARY </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PAID TWICE A MONTH</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (WHEN EXEMPT)</t>
+    </r>
+  </si>
+  <si>
+    <t>(non-exempt)</t>
+  </si>
+  <si>
+    <t>(exempt)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Non-exempt Hourly Wage</t>
+  </si>
+  <si>
+    <t>Exempt Weekly Wage</t>
+  </si>
+  <si>
+    <t>Exempt Biweekly Wage</t>
+  </si>
+  <si>
+    <t>Hours Accrued</t>
+  </si>
+  <si>
+    <t>Regular Hourly Wage</t>
+  </si>
+  <si>
+    <t>BOT Calculation</t>
+  </si>
 </sst>
 </file>
 
@@ -492,7 +523,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,8 +670,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -713,6 +757,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -736,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -827,7 +877,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -852,6 +901,12 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1166,11 +1221,1193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C526DF11-BA61-AF42-A736-34CDE4B01D07}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65" customWidth="1"/>
+    <col min="2" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="109" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E2" s="20">
+        <f t="shared" ref="E2:E7" si="0">D2+(1.22*C2)</f>
+        <v>52.78</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>25.5</v>
+      </c>
+      <c r="I2" s="13">
+        <v>25.5</v>
+      </c>
+      <c r="J2" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" si="0"/>
+        <v>53.695</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" ref="H3:I5" si="1">H2+0.75</f>
+        <v>26.25</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" si="1"/>
+        <v>26.25</v>
+      </c>
+      <c r="J3" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E4" s="20">
+        <f t="shared" si="0"/>
+        <v>54.61</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J4" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="D5" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
+        <v>55.524999999999999</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="1"/>
+        <v>27.75</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="1"/>
+        <v>27.75</v>
+      </c>
+      <c r="J5" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="0"/>
+        <v>52.78</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="8">
+        <v>26.5</v>
+      </c>
+      <c r="I6" s="13">
+        <v>26.5</v>
+      </c>
+      <c r="J6" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>25.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="0"/>
+        <v>53.695</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="8">
+        <v>27.25</v>
+      </c>
+      <c r="I7" s="13">
+        <v>27.25</v>
+      </c>
+      <c r="J7" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E8" s="20">
+        <f>D8+(1.22*C8)</f>
+        <v>68.36</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="8">
+        <v>35</v>
+      </c>
+      <c r="I8" s="13">
+        <v>35</v>
+      </c>
+      <c r="J8" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E9" s="20">
+        <f>D9+(1.22*C9)</f>
+        <v>64.09</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="I9" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="J9" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E10" s="20">
+        <f>D10+(1.22*C10)</f>
+        <v>64.09</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="I10" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="J10" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E11" s="20">
+        <f>D11+(1.22*C11)</f>
+        <v>64.7</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="8">
+        <v>32</v>
+      </c>
+      <c r="I11" s="13">
+        <v>32</v>
+      </c>
+      <c r="J11" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E12" s="20">
+        <f>D12+(1.22*C12)</f>
+        <v>65.615000000000009</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <f>H11+0.75</f>
+        <v>32.75</v>
+      </c>
+      <c r="I12" s="13">
+        <f>I11+0.75</f>
+        <v>32.75</v>
+      </c>
+      <c r="J12" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E13" s="20">
+        <f>D13+(1.22*C13)</f>
+        <v>66.53</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" ref="H13:I15" si="2">H12+0.75</f>
+        <v>33.5</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" si="2"/>
+        <v>33.5</v>
+      </c>
+      <c r="J13" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="D14" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E14" s="20">
+        <f>D14+(1.22*C14)</f>
+        <v>67.445000000000007</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="2"/>
+        <v>34.25</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" si="2"/>
+        <v>34.25</v>
+      </c>
+      <c r="J14" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4">
+        <v>64.7</v>
+      </c>
+      <c r="E15" s="20">
+        <f>D15+(1.22*C15)</f>
+        <v>68.36</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="J15" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>14.03</v>
+      </c>
+      <c r="E16" s="20">
+        <f>D16</f>
+        <v>14.03</v>
+      </c>
+      <c r="F16" s="28"/>
+      <c r="G16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="8">
+        <v>31.5</v>
+      </c>
+      <c r="I16" s="13">
+        <v>31.5</v>
+      </c>
+      <c r="J16" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>31.57</v>
+      </c>
+      <c r="E17" s="20">
+        <f>D17</f>
+        <v>31.57</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="9">
+        <v>15.5</v>
+      </c>
+      <c r="I17" s="9">
+        <v>15.5</v>
+      </c>
+      <c r="J17" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17.75</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="21">
+        <v>0</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <v>17.75</v>
+      </c>
+      <c r="J18" s="59">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32E492D-C4B3-2C44-ACDF-1157B3E6EBBA}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="37">
+        <v>36.06</v>
+      </c>
+      <c r="C2" s="37">
+        <v>1538.46</v>
+      </c>
+      <c r="D2" s="37">
+        <v>0</v>
+      </c>
+      <c r="E2" s="57">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="37">
+        <v>38.46</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0</v>
+      </c>
+      <c r="D3" s="37">
+        <v>3125</v>
+      </c>
+      <c r="E3" s="57">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381C0FA-6B24-4E3A-9946-7706E839421C}">
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
+      <c r="A1" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="37">
+        <v>36.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="37">
+        <v>38.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="37"/>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="37">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>1538.46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="46">
+        <v>27.25</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="46"/>
+      <c r="C19" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="46">
+        <v>27.25</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="46"/>
+      <c r="C21" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="46">
+        <v>25.5</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="46"/>
+      <c r="C23" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="46"/>
+      <c r="C24" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="46"/>
+      <c r="C25" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="46">
+        <v>26.25</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="46"/>
+      <c r="C27" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="46"/>
+      <c r="C28" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="46">
+        <v>25.5</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="46"/>
+      <c r="C30" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="46"/>
+      <c r="C31" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="46">
+        <v>31.5</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="46"/>
+      <c r="C33" s="44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="46"/>
+      <c r="C34" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="46">
+        <v>25.5</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="46">
+        <v>32</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="46">
+        <v>25.5</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="46">
+        <v>28.5</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="46"/>
+      <c r="C39" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="46"/>
+      <c r="C40" s="44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="46">
+        <v>34.25</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="46">
+        <v>33</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="46">
+        <v>31.5</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="46"/>
+      <c r="C44" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="46">
+        <v>30.25</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="46"/>
+      <c r="C46" s="44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="46">
+        <v>31.5</v>
+      </c>
+      <c r="C47" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="46">
+        <v>28.5</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="45"/>
+      <c r="C49" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A12:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C24E54-EF21-466C-824B-15C0DA37549E}">
   <dimension ref="A1:I359"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E37"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,31 +2437,31 @@
         <v>13</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>33</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
     </row>
@@ -1403,15 +2640,15 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15"/>
     </row>
@@ -1500,15 +2737,15 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
@@ -1661,15 +2898,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
       <c r="H19" s="16"/>
       <c r="I19" s="15"/>
     </row>
@@ -1702,15 +2939,15 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
+      <c r="A21" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="16"/>
       <c r="I21" s="15"/>
     </row>
@@ -1766,97 +3003,105 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
+      <c r="A24" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
       <c r="E25" s="39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I28" s="26"/>
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1872,21 +3117,21 @@
       <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
+      <c r="A30" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1894,7 +3139,7 @@
         <v>16.18</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F31" s="28">
         <v>30</v>
@@ -1909,7 +3154,7 @@
     </row>
     <row r="32" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1917,7 +3162,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F32" s="28">
         <v>30</v>
@@ -1932,14 +3177,14 @@
     </row>
     <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4">
         <v>30</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F33" s="28">
         <v>16.18</v>
@@ -1948,7 +3193,7 @@
         <v>97153</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I33" s="26"/>
     </row>
@@ -1957,7 +3202,7 @@
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
       <c r="D34" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E34" s="33"/>
       <c r="F34" s="33"/>
@@ -1967,7 +3212,7 @@
     </row>
     <row r="35" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1979,38 +3224,40 @@
         <v>0</v>
       </c>
       <c r="G35" s="43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I35" s="38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
+      <c r="A36" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
     </row>
     <row r="37" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
+      <c r="A37" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="29"/>
       <c r="G37" s="24"/>
       <c r="H37" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I37" s="11" t="s">
         <v>35</v>
@@ -2998,1152 +4245,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C526DF11-BA61-AF42-A736-34CDE4B01D07}">
-  <dimension ref="A1:I26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="65" customWidth="1"/>
-    <col min="2" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="151" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E2" s="20">
-        <f t="shared" ref="E2:E7" si="0">D2+(1.22*C2)</f>
-        <v>52.78</v>
-      </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8">
-        <v>25.5</v>
-      </c>
-      <c r="I2" s="13">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D3" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E3" s="20">
-        <f t="shared" si="0"/>
-        <v>53.695</v>
-      </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:I5" si="1">H2+0.75</f>
-        <v>26.25</v>
-      </c>
-      <c r="I3" s="13">
-        <f t="shared" si="1"/>
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E4" s="20">
-        <f t="shared" si="0"/>
-        <v>54.61</v>
-      </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="I4" s="13">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2.25</v>
-      </c>
-      <c r="D5" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E5" s="20">
-        <f t="shared" si="0"/>
-        <v>55.524999999999999</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="8">
-        <f t="shared" si="1"/>
-        <v>27.75</v>
-      </c>
-      <c r="I5" s="13">
-        <f t="shared" si="1"/>
-        <v>27.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E6" s="20">
-        <f t="shared" si="0"/>
-        <v>52.78</v>
-      </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="8">
-        <v>26.5</v>
-      </c>
-      <c r="I6" s="13">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D7" s="4">
-        <v>52.78</v>
-      </c>
-      <c r="E7" s="20">
-        <f t="shared" si="0"/>
-        <v>53.695</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="8">
-        <v>27.25</v>
-      </c>
-      <c r="I7" s="13">
-        <v>27.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E8" s="20">
-        <f>D8+(1.22*C8)</f>
-        <v>68.36</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="8">
-        <v>35</v>
-      </c>
-      <c r="I8" s="13">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="D9" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E9" s="20">
-        <f>D9+(1.22*C9)</f>
-        <v>64.09</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="I9" s="13">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E10" s="20">
-        <f>D10+(1.22*C10)</f>
-        <v>64.09</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="I10" s="13">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E11" s="20">
-        <f>D11+(1.22*C11)</f>
-        <v>64.7</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="8">
-        <v>32</v>
-      </c>
-      <c r="I11" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E12" s="20">
-        <f>D12+(1.22*C12)</f>
-        <v>65.615000000000009</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="8">
-        <f>H11+0.75</f>
-        <v>32.75</v>
-      </c>
-      <c r="I12" s="13">
-        <f>I11+0.75</f>
-        <v>32.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D13" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E13" s="20">
-        <f>D13+(1.22*C13)</f>
-        <v>66.53</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="8">
-        <f t="shared" ref="H13:I15" si="2">H12+0.75</f>
-        <v>33.5</v>
-      </c>
-      <c r="I13" s="13">
-        <f t="shared" si="2"/>
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2.25</v>
-      </c>
-      <c r="D14" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E14" s="20">
-        <f>D14+(1.22*C14)</f>
-        <v>67.445000000000007</v>
-      </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" si="2"/>
-        <v>34.25</v>
-      </c>
-      <c r="I14" s="13">
-        <f t="shared" si="2"/>
-        <v>34.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3">
-        <v>32</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4">
-        <v>64.7</v>
-      </c>
-      <c r="E15" s="20">
-        <f>D15+(1.22*C15)</f>
-        <v>68.36</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="8">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="I15" s="13">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>14.03</v>
-      </c>
-      <c r="E16" s="20">
-        <f>D16</f>
-        <v>14.03</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="I16" s="13">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>31.57</v>
-      </c>
-      <c r="E17" s="20">
-        <f>D17</f>
-        <v>31.57</v>
-      </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="9">
-        <v>15.5</v>
-      </c>
-      <c r="I17" s="9">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="3">
-        <v>17.75</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="21">
-        <v>0</v>
-      </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10">
-        <v>17.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" s="8">
-        <v>0</v>
-      </c>
-      <c r="I22" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="39">
-        <v>120</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="8">
-        <v>120</v>
-      </c>
-      <c r="I23" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381C0FA-6B24-4E3A-9946-7706E839421C}">
-  <dimension ref="A1:I50"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="104" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-    </row>
-    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="37">
-        <v>36.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="37">
-        <v>38.46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="37">
-        <v>3125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
-        <v>1538.46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="46">
-        <v>27.25</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="46"/>
-      <c r="C19" s="44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="46">
-        <v>27.25</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="46"/>
-      <c r="C21" s="44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="46">
-        <v>25.5</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="46"/>
-      <c r="C23" s="44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="46"/>
-      <c r="C24" s="44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="46"/>
-      <c r="C25" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="46">
-        <v>26.25</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="46"/>
-      <c r="C27" s="44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="46"/>
-      <c r="C28" s="44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="46">
-        <v>25.5</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="46"/>
-      <c r="C30" s="44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="46"/>
-      <c r="C31" s="44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="46">
-        <v>31.5</v>
-      </c>
-      <c r="C32" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="46"/>
-      <c r="C33" s="44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="46"/>
-      <c r="C34" s="44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="46">
-        <v>25.5</v>
-      </c>
-      <c r="C35" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="46">
-        <v>32</v>
-      </c>
-      <c r="C36" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="46">
-        <v>25.5</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="46">
-        <v>28.5</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="46"/>
-      <c r="C39" s="44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="46"/>
-      <c r="C40" s="44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="46">
-        <v>34.25</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="46">
-        <v>33</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="46">
-        <v>31.5</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="46"/>
-      <c r="C44" s="44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="46">
-        <v>30.25</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="46"/>
-      <c r="C46" s="44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="46">
-        <v>31.5</v>
-      </c>
-      <c r="C47" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="46">
-        <v>28.5</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D48" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="45"/>
-      <c r="C49" s="44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="45"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A12:I12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fourth commit with payroll functions in ipynb
</commit_message>
<xml_diff>
--- a/billing.xlsx
+++ b/billing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haosenhe/PyFolder/Programs/nova-data-processing-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8586DB16-48D3-B94E-A04D-94FE0F16EFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55202FA1-AB77-6B47-A774-423153F8F7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{2580F89A-B4FE-4711-8C11-BBD44F6FB879}"/>
   </bookViews>
@@ -506,13 +506,13 @@
     <t>Exempt Biweekly Wage</t>
   </si>
   <si>
-    <t>Hours Accrued</t>
-  </si>
-  <si>
     <t>Regular Hourly Wage</t>
   </si>
   <si>
     <t>BOT Calculation</t>
+  </si>
+  <si>
+    <t>Accrue Rate</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1225,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1259,13 +1259,13 @@
         <v>33</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="58" t="s">
         <v>113</v>
-      </c>
-      <c r="J1" s="58" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1817,7 +1817,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1843,7 +1843,7 @@
         <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381C0FA-6B24-4E3A-9946-7706E839421C}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="104" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="104" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2406,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C24E54-EF21-466C-824B-15C0DA37549E}">
   <dimension ref="A1:I359"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
basic payroll processor completed
</commit_message>
<xml_diff>
--- a/billing.xlsx
+++ b/billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haosenhe/PyFolder/Programs/nova-data-processing-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55202FA1-AB77-6B47-A774-423153F8F7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AEEFAB-7675-124E-8192-9B614B7762F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{2580F89A-B4FE-4711-8C11-BBD44F6FB879}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2580F89A-B4FE-4711-8C11-BBD44F6FB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-manager Rates" sheetId="3" r:id="rId1"/>
@@ -509,10 +509,10 @@
     <t>Regular Hourly Wage</t>
   </si>
   <si>
-    <t>BOT Calculation</t>
-  </si>
-  <si>
     <t>Accrue Rate</t>
+  </si>
+  <si>
+    <t>BOT Hourly Wage</t>
   </si>
 </sst>
 </file>
@@ -877,6 +877,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -895,18 +907,6 @@
     <xf numFmtId="164" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C526DF11-BA61-AF42-A736-34CDE4B01D07}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1262,10 +1262,10 @@
         <v>111</v>
       </c>
       <c r="I1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="50" t="s">
         <v>112</v>
-      </c>
-      <c r="J1" s="58" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
       <c r="I2" s="13">
         <v>25.5</v>
       </c>
-      <c r="J2" s="59">
+      <c r="J2" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
         <f t="shared" si="1"/>
         <v>26.25</v>
       </c>
-      <c r="J3" s="59">
+      <c r="J3" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J4" s="59">
+      <c r="J4" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
         <f t="shared" si="1"/>
         <v>27.75</v>
       </c>
-      <c r="J5" s="59">
+      <c r="J5" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       <c r="I6" s="13">
         <v>26.5</v>
       </c>
-      <c r="J6" s="59">
+      <c r="J6" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
       <c r="I7" s="13">
         <v>27.25</v>
       </c>
-      <c r="J7" s="59">
+      <c r="J7" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1474,7 +1474,7 @@
         <v>64.7</v>
       </c>
       <c r="E8" s="20">
-        <f>D8+(1.22*C8)</f>
+        <f t="shared" ref="E8:E15" si="2">D8+(1.22*C8)</f>
         <v>68.36</v>
       </c>
       <c r="F8" s="28"/>
@@ -1487,7 +1487,7 @@
       <c r="I8" s="13">
         <v>35</v>
       </c>
-      <c r="J8" s="59">
+      <c r="J8" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1505,7 +1505,7 @@
         <v>64.7</v>
       </c>
       <c r="E9" s="20">
-        <f>D9+(1.22*C9)</f>
+        <f t="shared" si="2"/>
         <v>64.09</v>
       </c>
       <c r="F9" s="28"/>
@@ -1518,7 +1518,7 @@
       <c r="I9" s="13">
         <v>31.5</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
         <v>64.7</v>
       </c>
       <c r="E10" s="20">
-        <f>D10+(1.22*C10)</f>
+        <f t="shared" si="2"/>
         <v>64.09</v>
       </c>
       <c r="F10" s="28"/>
@@ -1549,7 +1549,7 @@
       <c r="I10" s="13">
         <v>31.5</v>
       </c>
-      <c r="J10" s="59">
+      <c r="J10" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
         <v>64.7</v>
       </c>
       <c r="E11" s="20">
-        <f>D11+(1.22*C11)</f>
+        <f t="shared" si="2"/>
         <v>64.7</v>
       </c>
       <c r="F11" s="28"/>
@@ -1580,7 +1580,7 @@
       <c r="I11" s="13">
         <v>32</v>
       </c>
-      <c r="J11" s="59">
+      <c r="J11" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1598,7 +1598,7 @@
         <v>64.7</v>
       </c>
       <c r="E12" s="20">
-        <f>D12+(1.22*C12)</f>
+        <f t="shared" si="2"/>
         <v>65.615000000000009</v>
       </c>
       <c r="F12" s="28"/>
@@ -1613,7 +1613,7 @@
         <f>I11+0.75</f>
         <v>32.75</v>
       </c>
-      <c r="J12" s="59">
+      <c r="J12" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
         <v>64.7</v>
       </c>
       <c r="E13" s="20">
-        <f>D13+(1.22*C13)</f>
+        <f t="shared" si="2"/>
         <v>66.53</v>
       </c>
       <c r="F13" s="28"/>
@@ -1639,14 +1639,14 @@
         <v>5</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" ref="H13:I15" si="2">H12+0.75</f>
+        <f t="shared" ref="H13:I15" si="3">H12+0.75</f>
         <v>33.5</v>
       </c>
       <c r="I13" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.5</v>
       </c>
-      <c r="J13" s="59">
+      <c r="J13" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1664,7 +1664,7 @@
         <v>64.7</v>
       </c>
       <c r="E14" s="20">
-        <f>D14+(1.22*C14)</f>
+        <f t="shared" si="2"/>
         <v>67.445000000000007</v>
       </c>
       <c r="F14" s="28"/>
@@ -1672,14 +1672,14 @@
         <v>6</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.25</v>
       </c>
       <c r="I14" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34.25</v>
       </c>
-      <c r="J14" s="59">
+      <c r="J14" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
         <v>64.7</v>
       </c>
       <c r="E15" s="20">
-        <f>D15+(1.22*C15)</f>
+        <f t="shared" si="2"/>
         <v>68.36</v>
       </c>
       <c r="F15" s="28"/>
@@ -1705,14 +1705,14 @@
         <v>7</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="I15" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="J15" s="59">
+      <c r="J15" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1743,7 +1743,7 @@
       <c r="I16" s="13">
         <v>31.5</v>
       </c>
-      <c r="J16" s="59">
+      <c r="J16" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
       <c r="I17" s="9">
         <v>15.5</v>
       </c>
-      <c r="J17" s="59">
+      <c r="J17" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
       <c r="I18" s="10">
         <v>17.75</v>
       </c>
-      <c r="J18" s="59">
+      <c r="J18" s="51">
         <v>0.04</v>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1843,40 +1843,40 @@
         <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="48" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="37">
         <v>36.06</v>
       </c>
-      <c r="C2" s="37">
-        <v>1538.46</v>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2" s="37">
-        <v>0</v>
-      </c>
-      <c r="E2" s="57">
+        <v>3125</v>
+      </c>
+      <c r="E2" s="49">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="37">
         <v>38.46</v>
       </c>
       <c r="C3" s="37">
+        <v>1538.46</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3" s="37">
-        <v>3125</v>
-      </c>
-      <c r="E3" s="57">
+      <c r="E3" s="49">
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1902,17 +1902,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.3">
@@ -1922,17 +1922,17 @@
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1954,17 +1954,17 @@
       <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1980,17 +1980,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2453,15 +2453,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="14"/>
       <c r="I2" s="15"/>
     </row>
@@ -2640,15 +2640,15 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="16"/>
       <c r="I9" s="15"/>
     </row>
@@ -2737,15 +2737,15 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
@@ -2898,15 +2898,15 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="16"/>
       <c r="I19" s="15"/>
     </row>
@@ -2939,15 +2939,15 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="16"/>
       <c r="I21" s="15"/>
     </row>
@@ -3003,15 +3003,15 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
@@ -3117,15 +3117,15 @@
       <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
     </row>
@@ -3234,26 +3234,26 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="29"/>
       <c r="G37" s="24"/>
       <c r="H37" s="12" t="s">

</xml_diff>